<commit_message>
Added error if resume not added to db, updated spread of requirements
</commit_message>
<xml_diff>
--- a/Report Spreadsheet.xlsx
+++ b/Report Spreadsheet.xlsx
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
   <si>
     <t>Administrator Reports</t>
   </si>
@@ -339,9 +339,6 @@
     <t>TODO: fill in the rest</t>
   </si>
   <si>
-    <t>Update Resume: Allow seeker to update resume**</t>
-  </si>
-  <si>
     <t>Note that we have expanded this to allow multiple resumes to be uploaded and modified by the user</t>
   </si>
   <si>
@@ -435,9 +432,6 @@
     <t>Not Implemented</t>
   </si>
   <si>
-    <t>not sure if we should implement?</t>
-  </si>
-  <si>
     <t>Do we need more search criteria?</t>
   </si>
   <si>
@@ -448,6 +442,18 @@
   </si>
   <si>
     <t>Work Experience: displayed in descending order by start date</t>
+  </si>
+  <si>
+    <t>Update Resume: Allow seeker to update resume</t>
+  </si>
+  <si>
+    <t>idk how this is useful</t>
+  </si>
+  <si>
+    <t>not complete</t>
+  </si>
+  <si>
+    <t>Should we fix this?</t>
   </si>
 </sst>
 </file>
@@ -564,7 +570,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -590,6 +596,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -885,7 +893,7 @@
   <dimension ref="A1:C128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -897,13 +905,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
@@ -916,133 +924,147 @@
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>54</v>
+      <c r="B3" s="11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>52</v>
+      <c r="B4" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>52</v>
+        <v>40</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="B13" s="12"/>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
         <v>45</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
         <v>47</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1162,74 +1184,104 @@
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B55" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>10</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1255,16 +1307,25 @@
       <c r="A70" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B70" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B71" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B72" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="C72" t="s">
         <v>8</v>
       </c>
@@ -1273,21 +1334,33 @@
       <c r="A73" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B73" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B74" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="75" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B75" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B76" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
@@ -1303,64 +1376,67 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B81" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -1381,10 +1457,10 @@
     </row>
     <row r="100" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -1407,12 +1483,12 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>